<commit_message>
Synonym list updated, expanded and sorted alphabetically in reference by HELP >filename
</commit_message>
<xml_diff>
--- a/info/BLUESKY-COMMAND-TABLE.xlsx
+++ b/info/BLUESKY-COMMAND-TABLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="316">
   <si>
     <t>Command</t>
   </si>
@@ -953,6 +953,15 @@
   </si>
   <si>
     <t>Equivalent command</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
+  </si>
+  <si>
+    <t>LOAD</t>
   </si>
 </sst>
 </file>
@@ -1842,10 +1851,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3027,47 +3036,47 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>178</v>
+        <v>47</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>104</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>157</v>
@@ -3075,55 +3084,55 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>129</v>
+        <v>291</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>296</v>
+        <v>309</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>170</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>160</v>
+        <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>47</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>129</v>
@@ -3131,58 +3140,58 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>242</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>104</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>101</v>
+        <v>188</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -3195,7 +3204,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>132</v>
@@ -3203,18 +3212,42 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>291</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Synonymes description in command reference and synonyms in HELP
</commit_message>
<xml_diff>
--- a/info/BLUESKY-COMMAND-TABLE.xlsx
+++ b/info/BLUESKY-COMMAND-TABLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="316">
   <si>
     <t>Command</t>
   </si>
@@ -1480,7 +1480,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1505,6 +1505,15 @@
     </xf>
     <xf numFmtId="49" fontId="16" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1853,8 +1862,8 @@
   </sheetPr>
   <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3033,6 +3042,10 @@
       <c r="B88" s="7" t="s">
         <v>312</v>
       </c>
+      <c r="C88" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" s="10"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
@@ -3041,6 +3054,10 @@
       <c r="B89" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C89" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
@@ -3049,6 +3066,10 @@
       <c r="B90" s="1" t="s">
         <v>104</v>
       </c>
+      <c r="C90" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D90" s="1"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
@@ -3057,6 +3078,10 @@
       <c r="B91" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="C91" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
@@ -3065,6 +3090,10 @@
       <c r="B92" s="1" t="s">
         <v>170</v>
       </c>
+      <c r="C92" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
@@ -3073,6 +3102,10 @@
       <c r="B93" s="1" t="s">
         <v>167</v>
       </c>
+      <c r="C93" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
@@ -3081,6 +3114,10 @@
       <c r="B94" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="C94" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
@@ -3089,6 +3126,10 @@
       <c r="B95" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="C95" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
@@ -3097,158 +3138,238 @@
       <c r="B96" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C96" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D96" s="1"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>301</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D97" s="1"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>309</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>288</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C99" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>295</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C100" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>306</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C101" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>299</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C102" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>315</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C103" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>313</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C104" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>300</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C105" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D105" s="1"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>303</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C106" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D106" s="1"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>290</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C107" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D107" s="1"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>293</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C108" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D108" s="1"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>307</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C109" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D109" s="1"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>304</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C110" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D110" s="1"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>291</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C111" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D111" s="1"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>297</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C112" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D112" s="1"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>289</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C113" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D113" s="1"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>302</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C114" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D114" s="1"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>305</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="C115" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D115" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
HELP PDF command added
</commit_message>
<xml_diff>
--- a/info/BLUESKY-COMMAND-TABLE.xlsx
+++ b/info/BLUESKY-COMMAND-TABLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="319">
   <si>
     <t>Command</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Show help in a command or write list of commands to file</t>
   </si>
   <si>
-    <t>HELP [command] / &gt;filename</t>
-  </si>
-  <si>
     <t>[txt]</t>
   </si>
   <si>
@@ -968,6 +965,12 @@
   </si>
   <si>
     <t>Toggle aircraft trails on/off</t>
+  </si>
+  <si>
+    <t>HELP [command]  or PDF or &gt;filename</t>
+  </si>
+  <si>
+    <t>Show help on a command, a pdf or write commands to file</t>
   </si>
 </sst>
 </file>
@@ -1881,8 +1884,8 @@
   </sheetPr>
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1909,83 +1912,83 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -1993,16 +1996,16 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2021,13 +2024,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
@@ -2035,69 +2038,69 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="D12" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
@@ -2105,44 +2108,44 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D16" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>151</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -2161,83 +2164,83 @@
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>187</v>
-      </c>
       <c r="D21" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="D22" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>270</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="5" t="s">
         <v>212</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>213</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>13</v>
@@ -2245,16 +2248,16 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -2273,44 +2276,44 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="D28" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D29" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -2318,39 +2321,39 @@
         <v>47</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>318</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="C32" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>233</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -2369,16 +2372,16 @@
     </row>
     <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -2397,58 +2400,58 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="D38" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -2467,13 +2470,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>27</v>
@@ -2481,70 +2484,70 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="D43" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>242</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="D45" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="C46" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>251</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
@@ -2563,16 +2566,16 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="D49" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -2591,27 +2594,27 @@
     </row>
     <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="D51" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="C52" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>27</v>
@@ -2619,27 +2622,27 @@
     </row>
     <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="D53" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C54" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="1"/>
     </row>
@@ -2657,114 +2660,114 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="C56" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>223</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>230</v>
-      </c>
       <c r="D57" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="C58" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>182</v>
-      </c>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="C60" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="D61" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="D62" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>248</v>
-      </c>
       <c r="D63" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -2797,13 +2800,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>13</v>
@@ -2811,69 +2814,69 @@
     </row>
     <row r="67" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="D67" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="D68" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C69" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C69" s="5" t="s">
+      <c r="D69" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="D70" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>27</v>
@@ -2881,16 +2884,16 @@
     </row>
     <row r="72" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="D72" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -2907,151 +2910,151 @@
     </row>
     <row r="74" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="C75" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="D75" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>258</v>
-      </c>
       <c r="D76" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C77" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C77" s="5" t="s">
+      <c r="D77" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="C78" s="5" t="s">
-        <v>273</v>
-      </c>
       <c r="D78" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C79" s="5" t="s">
+      <c r="D79" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C80" s="5" t="s">
+      <c r="D80" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>245</v>
-      </c>
       <c r="D81" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="D82" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="D83" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="86" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B86" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>303</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>1</v>
@@ -3060,7 +3063,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>47</v>
@@ -3072,115 +3075,115 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="D88" s="1"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="D90" s="1"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B91" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C91" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>160</v>
       </c>
       <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C94" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C95" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>28</v>
@@ -3192,193 +3195,193 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C98" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C99" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="D99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C101" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C102" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C103" s="9" t="s">
         <v>234</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>235</v>
       </c>
       <c r="D103" s="1"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C104" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="D104" s="1"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>181</v>
       </c>
       <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C106" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>129</v>
       </c>
       <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C107" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C108" s="9" t="s">
         <v>126</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C109" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C109" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C110" s="9" t="s">
         <v>152</v>
-      </c>
-      <c r="C110" s="9" t="s">
-        <v>153</v>
       </c>
       <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C111" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C112" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D112" s="1"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C113" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D113" s="1"/>
     </row>

</xml_diff>

<commit_message>
SAVE synonym in list
</commit_message>
<xml_diff>
--- a/info/BLUESKY-COMMAND-TABLE.xlsx
+++ b/info/BLUESKY-COMMAND-TABLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="320">
   <si>
     <t>Command</t>
   </si>
@@ -971,6 +971,9 @@
   </si>
   <si>
     <t>Show help on a command, a pdf or write commands to file</t>
+  </si>
+  <si>
+    <t>SAVE</t>
   </si>
 </sst>
 </file>
@@ -1882,10 +1885,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3315,55 +3318,55 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>126</v>
+        <v>40</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>98</v>
+        <v>152</v>
       </c>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>97</v>
@@ -3375,7 +3378,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>97</v>
@@ -3384,6 +3387,18 @@
         <v>98</v>
       </c>
       <c r="D113" s="1"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D114" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Next to LNAV, VNAV also activated when DEST is given
</commit_message>
<xml_diff>
--- a/info/BLUESKY-COMMAND-TABLE.xlsx
+++ b/info/BLUESKY-COMMAND-TABLE.xlsx
@@ -1887,7 +1887,7 @@
   </sheetPr>
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
@@ -2165,7 +2165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>165</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>261</v>
       </c>

</xml_diff>